<commit_message>
Enhance multi-language support and logging in Cutting Optimizer Pro
- Registered Arabic fonts and added RTL support for PDF and Excel exports in co.py.
- Updated export functions to handle translations dynamically based on selected language.
- Improved logging setup to store logs in the user's AppData directory.
- Added "Open Output Folder" functionality in the GUI for easier access to output files.
- Updated .gitignore to include new installer and spec files.
- Modified translations.json to include new keys for file operations and folder access.
- Incremented version to 1.2 in version.json to reflect new features and improvements.
</commit_message>
<xml_diff>
--- a/optimized_cutting_plan_facture.xlsx
+++ b/optimized_cutting_plan_facture.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="122">
   <si>
-    <t>Facture</t>
+    <t>Invoice</t>
   </si>
   <si>
     <t>Date: 18/12/2024</t>
@@ -25,22 +25,22 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Poids/ml (kg)</t>
-  </si>
-  <si>
-    <t>Long. Stock</t>
-  </si>
-  <si>
-    <t>QTE</t>
-  </si>
-  <si>
-    <t>Poids Total (kg)</t>
-  </si>
-  <si>
-    <t>Pourcentage</t>
-  </si>
-  <si>
-    <t>Prix Total</t>
+    <t>Weight/m (kg)</t>
+  </si>
+  <si>
+    <t>Stock Length</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>Total Weight (kg)</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Total Price</t>
   </si>
   <si>
     <t>PL10*160</t>
@@ -52,7 +52,7 @@
     <t>0.7%</t>
   </si>
   <si>
-    <t>11270.000</t>
+    <t>322.000</t>
   </si>
   <si>
     <t>PL10*153</t>
@@ -64,7 +64,7 @@
     <t>0.1%</t>
   </si>
   <si>
-    <t>1680.000</t>
+    <t>48.000</t>
   </si>
   <si>
     <t>PL10*100</t>
@@ -76,7 +76,7 @@
     <t>0.4%</t>
   </si>
   <si>
-    <t>6720.000</t>
+    <t>192.000</t>
   </si>
   <si>
     <t>PD54*13</t>
@@ -88,7 +88,7 @@
     <t>0.5%</t>
   </si>
   <si>
-    <t>7840.000</t>
+    <t>224.000</t>
   </si>
   <si>
     <t>D18</t>
@@ -97,7 +97,7 @@
     <t>0.400</t>
   </si>
   <si>
-    <t>1120.000</t>
+    <t>32.000</t>
   </si>
   <si>
     <t>PL10*250</t>
@@ -109,7 +109,7 @@
     <t>1.3%</t>
   </si>
   <si>
-    <t>20160.000</t>
+    <t>576.000</t>
   </si>
   <si>
     <t>PL10*60</t>
@@ -121,7 +121,7 @@
     <t>2.000</t>
   </si>
   <si>
-    <t>8400.000</t>
+    <t>240.000</t>
   </si>
   <si>
     <t>PL10*90</t>
@@ -130,7 +130,7 @@
     <t>1.300</t>
   </si>
   <si>
-    <t>910.000</t>
+    <t>26.000</t>
   </si>
   <si>
     <t>PL10*200</t>
@@ -142,7 +142,7 @@
     <t>0.3%</t>
   </si>
   <si>
-    <t>4340.000</t>
+    <t>124.000</t>
   </si>
   <si>
     <t>HEA140</t>
@@ -154,7 +154,7 @@
     <t>31.7%</t>
   </si>
   <si>
-    <t>486780.000</t>
+    <t>13908.000</t>
   </si>
   <si>
     <t>PL8*127</t>
@@ -166,7 +166,7 @@
     <t>PL8*147</t>
   </si>
   <si>
-    <t>840.000</t>
+    <t>24.000</t>
   </si>
   <si>
     <t>PL8*50</t>
@@ -175,7 +175,7 @@
     <t>0.200</t>
   </si>
   <si>
-    <t>980.000</t>
+    <t>28.000</t>
   </si>
   <si>
     <t>PL8*131</t>
@@ -184,7 +184,7 @@
     <t>2.100</t>
   </si>
   <si>
-    <t>1470.000</t>
+    <t>42.000</t>
   </si>
   <si>
     <t>PL8*145</t>
@@ -193,7 +193,7 @@
     <t>2.300</t>
   </si>
   <si>
-    <t>1610.000</t>
+    <t>46.000</t>
   </si>
   <si>
     <t>PL8*158</t>
@@ -202,7 +202,7 @@
     <t>2.500</t>
   </si>
   <si>
-    <t>875.000</t>
+    <t>25.000</t>
   </si>
   <si>
     <t>PL8*159</t>
@@ -214,7 +214,7 @@
     <t>1.000</t>
   </si>
   <si>
-    <t>6300.000</t>
+    <t>180.000</t>
   </si>
   <si>
     <t>PL8*125</t>
@@ -223,7 +223,7 @@
     <t>0.900</t>
   </si>
   <si>
-    <t>1260.000</t>
+    <t>36.000</t>
   </si>
   <si>
     <t>PL8*173</t>
@@ -232,7 +232,7 @@
     <t>1.900</t>
   </si>
   <si>
-    <t>1330.000</t>
+    <t>38.000</t>
   </si>
   <si>
     <t>PL8*209</t>
@@ -247,7 +247,7 @@
     <t>2.7%</t>
   </si>
   <si>
-    <t>41160.000</t>
+    <t>1176.000</t>
   </si>
   <si>
     <t>D27</t>
@@ -259,7 +259,7 @@
     <t>0.9%</t>
   </si>
   <si>
-    <t>14280.000</t>
+    <t>408.000</t>
   </si>
   <si>
     <t>IPE270</t>
@@ -271,7 +271,7 @@
     <t>20.5%</t>
   </si>
   <si>
-    <t>314895.000</t>
+    <t>8997.000</t>
   </si>
   <si>
     <t>UPN200</t>
@@ -283,7 +283,7 @@
     <t>21.0%</t>
   </si>
   <si>
-    <t>323155.000</t>
+    <t>9233.000</t>
   </si>
   <si>
     <t>L50*5</t>
@@ -295,7 +295,7 @@
     <t>2.2%</t>
   </si>
   <si>
-    <t>34370.000</t>
+    <t>982.000</t>
   </si>
   <si>
     <t>L60*6</t>
@@ -307,7 +307,7 @@
     <t>7.2%</t>
   </si>
   <si>
-    <t>111265.000</t>
+    <t>3179.000</t>
   </si>
   <si>
     <t>UPN160</t>
@@ -319,7 +319,7 @@
     <t>4.9%</t>
   </si>
   <si>
-    <t>75180.000</t>
+    <t>2148.000</t>
   </si>
   <si>
     <t>RHS90*70*2</t>
@@ -331,7 +331,7 @@
     <t>1.7%</t>
   </si>
   <si>
-    <t>26460.000</t>
+    <t>756.000</t>
   </si>
   <si>
     <t>UPN100</t>
@@ -343,7 +343,7 @@
     <t>0.6%</t>
   </si>
   <si>
-    <t>9555.000</t>
+    <t>273.000</t>
   </si>
   <si>
     <t>UPN120</t>
@@ -355,7 +355,7 @@
     <t>0.8%</t>
   </si>
   <si>
-    <t>11935.000</t>
+    <t>341.000</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -367,10 +367,10 @@
     <t>100%</t>
   </si>
   <si>
-    <t>1536325.000</t>
-  </si>
-  <si>
-    <t>TOTAL AJUSTE (+{0}%) (12.0%)</t>
+    <t>43895.000</t>
+  </si>
+  <si>
+    <t>ADJUSTED TOTAL (+{0}%) (12.0%)</t>
   </si>
   <si>
     <t>4916.240</t>
@@ -379,7 +379,7 @@
     <t>112%</t>
   </si>
   <si>
-    <t>1720684.000</t>
+    <t>49162.400</t>
   </si>
 </sst>
 </file>

</xml_diff>